<commit_message>
update specs of solar panel
</commit_message>
<xml_diff>
--- a/Projects/Solar_Powered_Battery/Docs/Solar_Panel_Specs.xlsx
+++ b/Projects/Solar_Powered_Battery/Docs/Solar_Panel_Specs.xlsx
@@ -1,16 +1,18 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21425"/>
   <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF91B06A-CE8E-45CC-80FB-0C67C25E71E7}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Output_Power" sheetId="1" r:id="rId1"/>
     <sheet name="Calculation" sheetId="2" r:id="rId2"/>
+    <sheet name="ToDo" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -20,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="95">
   <si>
     <t>Pout_max[W]</t>
   </si>
@@ -176,13 +178,145 @@
   </si>
   <si>
     <t>170mA</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>H/S</t>
+  </si>
+  <si>
+    <t>create a couter as soon as the sun is shining and turn on the pump at specific time</t>
+  </si>
+  <si>
+    <t>S</t>
+  </si>
+  <si>
+    <t>Create sleep configuration</t>
+  </si>
+  <si>
+    <t>H</t>
+  </si>
+  <si>
+    <t>How many solar panels</t>
+  </si>
+  <si>
+    <t>How much power is required</t>
+  </si>
+  <si>
+    <t>Use back to back PMOS as ideal diodes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Create logic for turning off one of the supplies </t>
+  </si>
+  <si>
+    <t>450mA</t>
+  </si>
+  <si>
+    <t>Calculation</t>
+  </si>
+  <si>
+    <t>Value</t>
+  </si>
+  <si>
+    <t>Unit</t>
+  </si>
+  <si>
+    <t>W</t>
+  </si>
+  <si>
+    <t>V</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>Variable</t>
+  </si>
+  <si>
+    <t>Battery_Cap</t>
+  </si>
+  <si>
+    <t>Ah</t>
+  </si>
+  <si>
+    <t>Battery_Discharge</t>
+  </si>
+  <si>
+    <t>h</t>
+  </si>
+  <si>
+    <t>Charge Current max (0.5CC)</t>
+  </si>
+  <si>
+    <t>2500mA</t>
+  </si>
+  <si>
+    <t>Charger_eff</t>
+  </si>
+  <si>
+    <t>Battery_Charging</t>
+  </si>
+  <si>
+    <t>Charger_Iout</t>
+  </si>
+  <si>
+    <t>Battery Charger</t>
+  </si>
+  <si>
+    <t>Load</t>
+  </si>
+  <si>
+    <t>Boost Converter</t>
+  </si>
+  <si>
+    <t>Battery</t>
+  </si>
+  <si>
+    <t>Buck Converter</t>
+  </si>
+  <si>
+    <t>Eff</t>
+  </si>
+  <si>
+    <t>Vin_min</t>
+  </si>
+  <si>
+    <t>Vin_max</t>
+  </si>
+  <si>
+    <t>Pout</t>
+  </si>
+  <si>
+    <t>P_max</t>
+  </si>
+  <si>
+    <t>I_max</t>
+  </si>
+  <si>
+    <t>Solar Panel</t>
+  </si>
+  <si>
+    <t>Vout_min</t>
+  </si>
+  <si>
+    <t>Vout_max</t>
+  </si>
+  <si>
+    <t>I_min</t>
+  </si>
+  <si>
+    <t>Iout_min</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="165" formatCode="0.000"/>
+  </numFmts>
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -190,13 +324,26 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -226,12 +373,45 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -247,9 +427,9 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="de-DE"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -286,7 +466,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="de-DE"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -629,7 +809,7 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-41FC-4065-8FD8-7B09B5829832}"/>
             </c:ext>
@@ -701,7 +881,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="de-DE"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="390092456"/>
@@ -763,7 +943,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="de-DE"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="390091672"/>
@@ -780,14 +960,14 @@
     </c:plotArea>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
-    <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+    <c:extLst>
       <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
         <c16r3:dataDisplayOptions16>
           <c16r3:dispNaAsBlank val="1"/>
         </c16r3:dataDisplayOptions16>
       </c:ext>
     </c:extLst>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -811,7 +991,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="de-DE"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -1398,7 +1578,7 @@
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{335F42FB-C32E-4F1A-A28F-21DAE6D43FE9}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{335F42FB-C32E-4F1A-A28F-21DAE6D43FE9}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1425,24 +1605,30 @@
     <xdr:from>
       <xdr:col>18</xdr:col>
       <xdr:colOff>392524</xdr:colOff>
-      <xdr:row>26</xdr:row>
+      <xdr:row>27</xdr:row>
       <xdr:rowOff>32655</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>20</xdr:col>
       <xdr:colOff>392524</xdr:colOff>
-      <xdr:row>31</xdr:row>
-      <xdr:rowOff>175530</xdr:rowOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="2" name="Rechteck 1"/>
+        <xdr:cNvPr id="2" name="Rechteck 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="15591703" y="4985655"/>
-          <a:ext cx="1524000" cy="1095375"/>
+          <a:off x="15594424" y="4985655"/>
+          <a:ext cx="1524000" cy="1072245"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1511,7 +1697,18 @@
                 <a:schemeClr val="tx1"/>
               </a:solidFill>
             </a:rPr>
-            <a:t>Pmax=1.4W</a:t>
+            <a:t>Iin: 280mA (50mA)</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="de-DE" sz="1100" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>Pmax:1.4W (200mW)</a:t>
           </a:r>
           <a:endParaRPr lang="de-DE" sz="1100">
             <a:solidFill>
@@ -1535,18 +1732,24 @@
     <xdr:from>
       <xdr:col>14</xdr:col>
       <xdr:colOff>96609</xdr:colOff>
-      <xdr:row>21</xdr:row>
+      <xdr:row>22</xdr:row>
       <xdr:rowOff>129268</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
       <xdr:colOff>20409</xdr:colOff>
-      <xdr:row>28</xdr:row>
+      <xdr:row>29</xdr:row>
       <xdr:rowOff>176893</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="3" name="Rechteck 2"/>
+        <xdr:cNvPr id="3" name="Rechteck 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000003000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -1597,6 +1800,26 @@
             </a:rPr>
             <a:t>Boost</a:t>
           </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1400">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>MT3608</a:t>
+          </a:r>
+          <a:endParaRPr lang="de-DE" sz="1400" b="0" i="0">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
         </a:p>
         <a:p>
           <a:pPr algn="l"/>
@@ -1725,23 +1948,29 @@
     <xdr:from>
       <xdr:col>16</xdr:col>
       <xdr:colOff>312963</xdr:colOff>
-      <xdr:row>13</xdr:row>
+      <xdr:row>14</xdr:row>
       <xdr:rowOff>81642</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
       <xdr:colOff>608895</xdr:colOff>
-      <xdr:row>15</xdr:row>
+      <xdr:row>16</xdr:row>
       <xdr:rowOff>20879</xdr:rowOff>
     </xdr:to>
     <xdr:grpSp>
       <xdr:nvGrpSpPr>
-        <xdr:cNvPr id="8" name="Gruppieren 7"/>
+        <xdr:cNvPr id="8" name="Gruppieren 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000008000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGrpSpPr/>
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="13990863" y="2558142"/>
+          <a:off x="13324941" y="2748642"/>
           <a:ext cx="295932" cy="320237"/>
           <a:chOff x="12079999" y="2647950"/>
           <a:chExt cx="295932" cy="320237"/>
@@ -1749,7 +1978,13 @@
       </xdr:grpSpPr>
       <xdr:sp macro="" textlink="">
         <xdr:nvSpPr>
-          <xdr:cNvPr id="5" name="Gleichschenkliges Dreieck 4"/>
+          <xdr:cNvPr id="5" name="Gleichschenkliges Dreieck 4">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000005000000}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
           <xdr:cNvSpPr/>
         </xdr:nvSpPr>
         <xdr:spPr>
@@ -1796,7 +2031,13 @@
       </xdr:sp>
       <xdr:cxnSp macro="">
         <xdr:nvCxnSpPr>
-          <xdr:cNvPr id="7" name="Gerader Verbinder 6"/>
+          <xdr:cNvPr id="7" name="Gerader Verbinder 6">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000007000000}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
           <xdr:cNvCxnSpPr/>
         </xdr:nvCxnSpPr>
         <xdr:spPr>
@@ -1835,23 +2076,29 @@
     <xdr:from>
       <xdr:col>16</xdr:col>
       <xdr:colOff>312963</xdr:colOff>
-      <xdr:row>24</xdr:row>
+      <xdr:row>25</xdr:row>
       <xdr:rowOff>81642</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
       <xdr:colOff>608895</xdr:colOff>
-      <xdr:row>26</xdr:row>
+      <xdr:row>27</xdr:row>
       <xdr:rowOff>20879</xdr:rowOff>
     </xdr:to>
     <xdr:grpSp>
       <xdr:nvGrpSpPr>
-        <xdr:cNvPr id="9" name="Gruppieren 8"/>
+        <xdr:cNvPr id="9" name="Gruppieren 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000009000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGrpSpPr/>
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="13990863" y="4653642"/>
+          <a:off x="13324941" y="4844142"/>
           <a:ext cx="295932" cy="320237"/>
           <a:chOff x="12079999" y="2647950"/>
           <a:chExt cx="295932" cy="320237"/>
@@ -1859,7 +2106,13 @@
       </xdr:grpSpPr>
       <xdr:sp macro="" textlink="">
         <xdr:nvSpPr>
-          <xdr:cNvPr id="10" name="Gleichschenkliges Dreieck 9"/>
+          <xdr:cNvPr id="10" name="Gleichschenkliges Dreieck 9">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-00000A000000}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
           <xdr:cNvSpPr/>
         </xdr:nvSpPr>
         <xdr:spPr>
@@ -1906,7 +2159,13 @@
       </xdr:sp>
       <xdr:cxnSp macro="">
         <xdr:nvCxnSpPr>
-          <xdr:cNvPr id="11" name="Gerader Verbinder 10"/>
+          <xdr:cNvPr id="11" name="Gerader Verbinder 10">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-00000B000000}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
           <xdr:cNvCxnSpPr/>
         </xdr:nvCxnSpPr>
         <xdr:spPr>
@@ -1945,18 +2204,24 @@
     <xdr:from>
       <xdr:col>16</xdr:col>
       <xdr:colOff>589029</xdr:colOff>
-      <xdr:row>14</xdr:row>
+      <xdr:row>15</xdr:row>
       <xdr:rowOff>51262</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>17</xdr:col>
       <xdr:colOff>749993</xdr:colOff>
-      <xdr:row>19</xdr:row>
+      <xdr:row>20</xdr:row>
       <xdr:rowOff>70436</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="13" name="Gewinkelte Verbindung 12"/>
+        <xdr:cNvPr id="13" name="Gewinkelte Verbindung 12">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-00000D000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvCxnSpPr>
           <a:stCxn id="5" idx="0"/>
           <a:endCxn id="28" idx="1"/>
@@ -1999,18 +2264,24 @@
     <xdr:from>
       <xdr:col>18</xdr:col>
       <xdr:colOff>122463</xdr:colOff>
-      <xdr:row>19</xdr:row>
+      <xdr:row>20</xdr:row>
       <xdr:rowOff>70436</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>22</xdr:col>
       <xdr:colOff>143914</xdr:colOff>
-      <xdr:row>26</xdr:row>
+      <xdr:row>27</xdr:row>
       <xdr:rowOff>23027</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="14" name="Gewinkelte Verbindung 13"/>
+        <xdr:cNvPr id="14" name="Gewinkelte Verbindung 13">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-00000E000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvCxnSpPr>
           <a:stCxn id="28" idx="3"/>
           <a:endCxn id="20" idx="0"/>
@@ -2018,7 +2289,7 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="15321642" y="3689936"/>
+          <a:off x="15323049" y="3689936"/>
           <a:ext cx="3069451" cy="1286091"/>
         </a:xfrm>
         <a:prstGeom prst="bentConnector2">
@@ -2051,18 +2322,24 @@
     <xdr:from>
       <xdr:col>16</xdr:col>
       <xdr:colOff>589029</xdr:colOff>
-      <xdr:row>19</xdr:row>
+      <xdr:row>20</xdr:row>
       <xdr:rowOff>70436</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>17</xdr:col>
       <xdr:colOff>749993</xdr:colOff>
-      <xdr:row>25</xdr:row>
+      <xdr:row>26</xdr:row>
       <xdr:rowOff>51262</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="17" name="Gewinkelte Verbindung 16"/>
+        <xdr:cNvPr id="17" name="Gewinkelte Verbindung 16">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000011000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvCxnSpPr>
           <a:stCxn id="10" idx="0"/>
           <a:endCxn id="28" idx="1"/>
@@ -2105,24 +2382,30 @@
     <xdr:from>
       <xdr:col>21</xdr:col>
       <xdr:colOff>182014</xdr:colOff>
-      <xdr:row>26</xdr:row>
+      <xdr:row>27</xdr:row>
       <xdr:rowOff>23027</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>23</xdr:col>
       <xdr:colOff>105814</xdr:colOff>
       <xdr:row>32</xdr:row>
-      <xdr:rowOff>1045</xdr:rowOff>
+      <xdr:rowOff>164224</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="20" name="Rechteck 19"/>
+        <xdr:cNvPr id="20" name="Rechteck 19">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000014000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="17667193" y="4976027"/>
-          <a:ext cx="1447800" cy="1121018"/>
+          <a:off x="17668600" y="4976027"/>
+          <a:ext cx="1447800" cy="1093697"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2187,7 +2470,34 @@
                 <a:schemeClr val="tx1"/>
               </a:solidFill>
             </a:rPr>
-            <a:t>Pmax=0.85W</a:t>
+            <a:t>Iin: 170mA</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="de-DE" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>Pmax:</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="de-DE" sz="1100" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t> </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="de-DE" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>0.85W</a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -2206,18 +2516,24 @@
     <xdr:from>
       <xdr:col>17</xdr:col>
       <xdr:colOff>749993</xdr:colOff>
-      <xdr:row>19</xdr:row>
+      <xdr:row>20</xdr:row>
       <xdr:rowOff>3201</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>18</xdr:col>
       <xdr:colOff>122463</xdr:colOff>
-      <xdr:row>19</xdr:row>
+      <xdr:row>20</xdr:row>
       <xdr:rowOff>137671</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="28" name="Rechteck 27"/>
+        <xdr:cNvPr id="28" name="Rechteck 27">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-00001C000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -2260,18 +2576,24 @@
     <xdr:from>
       <xdr:col>18</xdr:col>
       <xdr:colOff>122463</xdr:colOff>
-      <xdr:row>19</xdr:row>
+      <xdr:row>20</xdr:row>
       <xdr:rowOff>70436</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>19</xdr:col>
       <xdr:colOff>392524</xdr:colOff>
-      <xdr:row>26</xdr:row>
+      <xdr:row>27</xdr:row>
       <xdr:rowOff>32655</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="31" name="Gewinkelte Verbindung 30"/>
+        <xdr:cNvPr id="31" name="Gewinkelte Verbindung 30">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-00001F000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvCxnSpPr>
           <a:stCxn id="28" idx="3"/>
           <a:endCxn id="2" idx="0"/>
@@ -2279,7 +2601,7 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="15321642" y="3689936"/>
+          <a:off x="15324363" y="3689936"/>
           <a:ext cx="1032061" cy="1295719"/>
         </a:xfrm>
         <a:prstGeom prst="bentConnector2">
@@ -2313,17 +2635,23 @@
       <xdr:col>20</xdr:col>
       <xdr:colOff>392524</xdr:colOff>
       <xdr:row>29</xdr:row>
-      <xdr:rowOff>8843</xdr:rowOff>
+      <xdr:rowOff>187778</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>21</xdr:col>
       <xdr:colOff>182014</xdr:colOff>
       <xdr:row>29</xdr:row>
-      <xdr:rowOff>12036</xdr:rowOff>
+      <xdr:rowOff>188876</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="39" name="Gewinkelte Verbindung 38"/>
+        <xdr:cNvPr id="39" name="Gewinkelte Verbindung 38">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000027000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvCxnSpPr>
           <a:stCxn id="2" idx="3"/>
           <a:endCxn id="20" idx="1"/>
@@ -2331,8 +2659,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="17115703" y="5533343"/>
-          <a:ext cx="551490" cy="3193"/>
+          <a:off x="17117110" y="5521778"/>
+          <a:ext cx="551490" cy="1098"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -2364,18 +2692,24 @@
     <xdr:from>
       <xdr:col>16</xdr:col>
       <xdr:colOff>20409</xdr:colOff>
-      <xdr:row>25</xdr:row>
+      <xdr:row>26</xdr:row>
       <xdr:rowOff>51262</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
       <xdr:colOff>312963</xdr:colOff>
-      <xdr:row>25</xdr:row>
+      <xdr:row>26</xdr:row>
       <xdr:rowOff>57831</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="51" name="Gewinkelte Verbindung 50"/>
+        <xdr:cNvPr id="51" name="Gewinkelte Verbindung 50">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000033000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvCxnSpPr>
           <a:stCxn id="3" idx="3"/>
           <a:endCxn id="10" idx="3"/>
@@ -2416,18 +2750,24 @@
     <xdr:from>
       <xdr:col>9</xdr:col>
       <xdr:colOff>582386</xdr:colOff>
-      <xdr:row>21</xdr:row>
+      <xdr:row>22</xdr:row>
       <xdr:rowOff>129268</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
       <xdr:colOff>506186</xdr:colOff>
-      <xdr:row>28</xdr:row>
+      <xdr:row>29</xdr:row>
       <xdr:rowOff>176893</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="60" name="Rechteck 59"/>
+        <xdr:cNvPr id="60" name="Rechteck 59">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-00003C000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -2490,6 +2830,21 @@
             </a:rPr>
             <a:t> Char</a:t>
           </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="de-DE" sz="1400" b="0" i="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>TP4056</a:t>
+          </a:r>
           <a:endParaRPr lang="de-DE" sz="1400" b="0" i="0">
             <a:solidFill>
               <a:schemeClr val="tx1"/>
@@ -2512,7 +2867,7 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t>Vin=</a:t>
+            <a:t>Vin=4..5..8</a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -2527,7 +2882,7 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t>Iin=</a:t>
+            <a:t>Iin=0.5mA</a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -2559,9 +2914,21 @@
             </a:rPr>
             <a:t>Iout_max=</a:t>
           </a:r>
+          <a:r>
+            <a:rPr lang="de-DE" sz="1100" b="0" i="0">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>1A</a:t>
+          </a:r>
           <a:endParaRPr lang="de-DE" sz="1100">
             <a:solidFill>
-              <a:schemeClr val="tx1"/>
+              <a:srgbClr val="FF0000"/>
             </a:solidFill>
           </a:endParaRPr>
         </a:p>
@@ -2573,18 +2940,24 @@
     <xdr:from>
       <xdr:col>9</xdr:col>
       <xdr:colOff>572859</xdr:colOff>
-      <xdr:row>10</xdr:row>
+      <xdr:row>11</xdr:row>
       <xdr:rowOff>129268</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
       <xdr:colOff>496659</xdr:colOff>
-      <xdr:row>17</xdr:row>
+      <xdr:row>18</xdr:row>
       <xdr:rowOff>176893</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="78" name="Rechteck 77"/>
+        <xdr:cNvPr id="78" name="Rechteck 77">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-00004E000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -2634,6 +3007,32 @@
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
             <a:t>Buck</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1400">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>TD1583</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="de-DE" sz="1400" b="0" i="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>TPS54331</a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -2736,18 +3135,24 @@
     <xdr:from>
       <xdr:col>11</xdr:col>
       <xdr:colOff>496659</xdr:colOff>
-      <xdr:row>14</xdr:row>
+      <xdr:row>15</xdr:row>
       <xdr:rowOff>51262</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
       <xdr:colOff>312963</xdr:colOff>
-      <xdr:row>14</xdr:row>
+      <xdr:row>15</xdr:row>
       <xdr:rowOff>57831</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="79" name="Gewinkelte Verbindung 50"/>
+        <xdr:cNvPr id="79" name="Gewinkelte Verbindung 50">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-00004F000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvCxnSpPr>
           <a:stCxn id="78" idx="3"/>
           <a:endCxn id="5" idx="3"/>
@@ -2788,18 +3193,24 @@
     <xdr:from>
       <xdr:col>10</xdr:col>
       <xdr:colOff>534759</xdr:colOff>
-      <xdr:row>17</xdr:row>
+      <xdr:row>18</xdr:row>
       <xdr:rowOff>176893</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
       <xdr:colOff>544286</xdr:colOff>
-      <xdr:row>21</xdr:row>
+      <xdr:row>22</xdr:row>
       <xdr:rowOff>129268</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="82" name="Gewinkelte Verbindung 50"/>
+        <xdr:cNvPr id="82" name="Gewinkelte Verbindung 50">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000052000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvCxnSpPr>
           <a:stCxn id="78" idx="2"/>
           <a:endCxn id="60" idx="0"/>
@@ -2840,18 +3251,24 @@
     <xdr:from>
       <xdr:col>6</xdr:col>
       <xdr:colOff>142875</xdr:colOff>
-      <xdr:row>10</xdr:row>
+      <xdr:row>11</xdr:row>
       <xdr:rowOff>129268</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
       <xdr:colOff>496659</xdr:colOff>
-      <xdr:row>17</xdr:row>
+      <xdr:row>18</xdr:row>
       <xdr:rowOff>176893</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="87" name="Rechteck 86"/>
+        <xdr:cNvPr id="87" name="Rechteck 86">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000057000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -2933,15 +3350,6 @@
             </a:rPr>
             <a:t>Vout_min=?? (depends on the buck)</a:t>
           </a:r>
-          <a:endParaRPr lang="de-DE" sz="1100" b="0" i="0">
-            <a:solidFill>
-              <a:schemeClr val="tx1"/>
-            </a:solidFill>
-            <a:effectLst/>
-            <a:latin typeface="+mn-lt"/>
-            <a:ea typeface="+mn-ea"/>
-            <a:cs typeface="+mn-cs"/>
-          </a:endParaRPr>
         </a:p>
         <a:p>
           <a:pPr algn="l"/>
@@ -3026,29 +3434,35 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>496659</xdr:colOff>
-      <xdr:row>14</xdr:row>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>293754</xdr:colOff>
+      <xdr:row>15</xdr:row>
       <xdr:rowOff>57831</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
       <xdr:colOff>572859</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>57831</xdr:rowOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>60787</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="88" name="Gewinkelte Verbindung 50"/>
+        <xdr:cNvPr id="88" name="Gewinkelte Verbindung 50">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000058000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvCxnSpPr>
-          <a:stCxn id="87" idx="3"/>
+          <a:stCxn id="29" idx="0"/>
           <a:endCxn id="78" idx="1"/>
         </xdr:cNvCxnSpPr>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
-        <a:xfrm>
-          <a:off x="8078559" y="2724831"/>
-          <a:ext cx="838200" cy="0"/>
+        <a:xfrm flipV="1">
+          <a:off x="8637654" y="2724831"/>
+          <a:ext cx="279105" cy="2956"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -3080,18 +3494,24 @@
     <xdr:from>
       <xdr:col>11</xdr:col>
       <xdr:colOff>753834</xdr:colOff>
-      <xdr:row>21</xdr:row>
+      <xdr:row>22</xdr:row>
       <xdr:rowOff>129268</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
       <xdr:colOff>677634</xdr:colOff>
-      <xdr:row>28</xdr:row>
+      <xdr:row>29</xdr:row>
       <xdr:rowOff>176893</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="97" name="Rechteck 96"/>
+        <xdr:cNvPr id="97" name="Rechteck 96">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000061000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -3145,6 +3565,29 @@
         </a:p>
         <a:p>
           <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="de-DE" sz="1100" b="0" i="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>	</a:t>
+          </a:r>
+          <a:br>
+            <a:rPr lang="de-DE" sz="1100" b="0" i="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+          </a:br>
           <a:r>
             <a:rPr lang="de-DE" sz="1100" b="0" i="0">
               <a:solidFill>
@@ -3213,18 +3656,24 @@
     <xdr:from>
       <xdr:col>11</xdr:col>
       <xdr:colOff>506186</xdr:colOff>
-      <xdr:row>25</xdr:row>
+      <xdr:row>26</xdr:row>
       <xdr:rowOff>57831</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
       <xdr:colOff>753834</xdr:colOff>
-      <xdr:row>25</xdr:row>
+      <xdr:row>26</xdr:row>
       <xdr:rowOff>57831</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="98" name="Gewinkelte Verbindung 50"/>
+        <xdr:cNvPr id="98" name="Gewinkelte Verbindung 50">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000062000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvCxnSpPr>
           <a:stCxn id="60" idx="3"/>
           <a:endCxn id="97" idx="1"/>
@@ -3265,18 +3714,24 @@
     <xdr:from>
       <xdr:col>13</xdr:col>
       <xdr:colOff>677634</xdr:colOff>
-      <xdr:row>25</xdr:row>
+      <xdr:row>26</xdr:row>
       <xdr:rowOff>57831</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
       <xdr:colOff>96609</xdr:colOff>
-      <xdr:row>25</xdr:row>
+      <xdr:row>26</xdr:row>
       <xdr:rowOff>57831</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="101" name="Gewinkelte Verbindung 50"/>
+        <xdr:cNvPr id="101" name="Gewinkelte Verbindung 50">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000065000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvCxnSpPr>
           <a:stCxn id="97" idx="3"/>
           <a:endCxn id="3" idx="1"/>
@@ -3294,6 +3749,248 @@
           <a:solidFill>
             <a:schemeClr val="tx1"/>
           </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>17688</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>91167</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>313620</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>30404</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="27" name="Gruppieren 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FE9B4560-03B7-49D8-ABAA-6DF52D2E6FEC}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="7695666" y="2758167"/>
+          <a:ext cx="295932" cy="320237"/>
+          <a:chOff x="12079999" y="2647950"/>
+          <a:chExt cx="295932" cy="320237"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="29" name="Gleichschenkliges Dreieck 4">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{771D8A4A-94AB-4165-BC57-11AA9E434C28}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm rot="5400000">
+            <a:off x="12057913" y="2670036"/>
+            <a:ext cx="320237" cy="276066"/>
+          </a:xfrm>
+          <a:prstGeom prst="triangle">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:solidFill>
+            <a:schemeClr val="bg1"/>
+          </a:solidFill>
+          <a:ln>
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:endParaRPr lang="de-DE" sz="1100"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:cxnSp macro="">
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="30" name="Gerader Verbinder 6">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{148873E4-A367-4356-9A37-C2F4F6ED8066}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvCxnSpPr/>
+        </xdr:nvCxnSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="12375931" y="2647950"/>
+            <a:ext cx="0" cy="314325"/>
+          </a:xfrm>
+          <a:prstGeom prst="line">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:ln w="15875">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+      </xdr:cxnSp>
+    </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>496659</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>57831</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>17688</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>60787</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="32" name="Gewinkelte Verbindung 50">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{83F7249D-5EA2-4D24-849F-0879697C9CB5}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="29" idx="3"/>
+          <a:endCxn id="87" idx="3"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1" flipV="1">
+          <a:off x="8078559" y="2724831"/>
+          <a:ext cx="283029" cy="2956"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="12700">
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>19707</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>78828</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>525517</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>78828</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="22" name="Straight Arrow Connector 21">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B51CA21D-57CB-4ABB-84CD-BA74A5D962DE}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="15220293" y="3507828"/>
+          <a:ext cx="505810" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="25400">
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+          <a:tailEnd type="triangle"/>
         </a:ln>
       </xdr:spPr>
       <xdr:style>
@@ -3578,14 +4275,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B54"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13.28515625" bestFit="1" customWidth="1"/>
   </cols>
@@ -4100,225 +4797,633 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B27"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:S73"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J10" sqref="J10"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A34" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="A59" sqref="A59:C59"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="33.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.7109375" style="5" customWidth="1"/>
+    <col min="2" max="3" width="11.42578125" style="3"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="1"/>
+      <c r="B1" s="2"/>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="1">
+      <c r="B2" s="2">
         <v>18650</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="2" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
+      <c r="A4" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" s="2" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
+      <c r="A5" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B6" s="2" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B7" s="2" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B8" s="2" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B9" s="2" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="B10" s="2" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B11" s="1"/>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
+      <c r="B12" s="2"/>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="B13" s="2" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="B13" s="1" t="s">
+      <c r="B14" s="2" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="B15" s="2" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" s="1" t="s">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="B15" s="1" t="s">
+      <c r="B16" s="2" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" s="1" t="s">
+    <row r="17" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A17" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="B16" s="1" t="s">
+      <c r="B17" s="2" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" s="1" t="s">
+    <row r="18" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A18" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="B17" s="1" t="s">
+      <c r="B18" s="2" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" s="1" t="s">
+    <row r="19" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A19" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="B18" s="1" t="s">
+      <c r="B19" s="2" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" s="1" t="s">
+      <c r="S19" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="20" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A20" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="B19" s="1" t="s">
+      <c r="B20" s="2" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" s="1" t="s">
+    <row r="21" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A21" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="B20" s="1" t="s">
+      <c r="B21" s="2" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" s="1" t="s">
+    <row r="22" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A22" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="B21" s="1" t="s">
+      <c r="B22" s="2" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" s="1" t="s">
+    <row r="23" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A23" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="B22" s="1" t="s">
+      <c r="B23" s="2" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" s="1" t="s">
+    <row r="24" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A24" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="B23" s="1" t="s">
+      <c r="B24" s="2" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" s="1" t="s">
+    <row r="25" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A25" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="B24" s="1" t="s">
+      <c r="B25" s="2" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25" s="1" t="s">
+    <row r="26" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A26" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="B25" s="1" t="s">
+      <c r="B26" s="2" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26" s="1" t="s">
+    <row r="27" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A27" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="B26" s="1" t="s">
+      <c r="B27" s="2" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A27" s="1" t="s">
+    <row r="28" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A28" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="B27" s="1" t="s">
+      <c r="B28" s="2" t="s">
         <v>29</v>
       </c>
     </row>
+    <row r="32" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A32" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="B32" s="6"/>
+      <c r="C32" s="6"/>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="B33" s="8"/>
+      <c r="C33" s="8"/>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="B34" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="C34" s="3" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="B35" s="7">
+        <f>1.4+0.85</f>
+        <v>2.25</v>
+      </c>
+      <c r="C35" s="3" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B36" s="7">
+        <v>5</v>
+      </c>
+      <c r="C36" s="3" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="B37" s="7">
+        <f>B35/B36</f>
+        <v>0.45</v>
+      </c>
+      <c r="C37" s="3" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B38" s="7"/>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="B39" s="8"/>
+      <c r="C39" s="8"/>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="B40" s="3">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="C41" s="3" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="C42" s="3" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A43" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="C43" s="3" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A44" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C44" s="3" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A45" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="B45" s="3">
+        <f>B43+B44</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A47" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="B47" s="8"/>
+      <c r="C47" s="8"/>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A48" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="B48" s="7">
+        <v>5</v>
+      </c>
+      <c r="C48" s="3" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A49" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="B49" s="7">
+        <f>B48*B40/B37</f>
+        <v>10</v>
+      </c>
+      <c r="C49" s="3" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A50" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="B50" s="7">
+        <f>B48/(B53*B54)</f>
+        <v>37.037037037037038</v>
+      </c>
+      <c r="C50" s="3" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B51" s="7"/>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A52" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="B52" s="8"/>
+      <c r="C52" s="8"/>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A53" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="B53" s="3">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A54" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="B54" s="3">
+        <v>0.15</v>
+      </c>
+      <c r="C54" s="3" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A59" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="B59" s="8"/>
+      <c r="C59" s="8"/>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A60" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="B60" s="3">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A61" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="C61" s="3" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A62" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="C62" s="3" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A63" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="C63" s="3" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A64" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C64" s="3" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A65" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="B65" s="3">
+        <f>B63+B64</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A66" s="12" t="s">
+        <v>94</v>
+      </c>
+      <c r="B66" s="7">
+        <f>B37</f>
+        <v>0.45</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A68" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="B68" s="8"/>
+      <c r="C68" s="8"/>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A69" s="10" t="s">
+        <v>91</v>
+      </c>
+      <c r="B69" s="9">
+        <v>0</v>
+      </c>
+      <c r="C69" s="9" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A70" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="B70" s="3">
+        <v>12</v>
+      </c>
+      <c r="C70" s="3" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A71" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="B71" s="3">
+        <v>1.5</v>
+      </c>
+      <c r="C71" s="3" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A72" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="B72" s="3">
+        <f>B71/B70</f>
+        <v>0.125</v>
+      </c>
+      <c r="C72" s="3" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A73" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="B73" s="11" t="e">
+        <f>B71/B69</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="C73" s="3" t="s">
+        <v>68</v>
+      </c>
+    </row>
   </sheetData>
+  <mergeCells count="7">
+    <mergeCell ref="A68:C68"/>
+    <mergeCell ref="A32:C32"/>
+    <mergeCell ref="A52:C52"/>
+    <mergeCell ref="A47:C47"/>
+    <mergeCell ref="A39:C39"/>
+    <mergeCell ref="A33:C33"/>
+    <mergeCell ref="A59:C59"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D62BF99-86B7-40C4-9F30-110AD341EFE4}">
+  <dimension ref="A1:B7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>53</v>
+      </c>
+      <c r="B2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>55</v>
+      </c>
+      <c r="B3" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>57</v>
+      </c>
+      <c r="B4" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>57</v>
+      </c>
+      <c r="B5" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>57</v>
+      </c>
+      <c r="B6" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>57</v>
+      </c>
+      <c r="B7" t="s">
+        <v>61</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
add simulation model solar panel
</commit_message>
<xml_diff>
--- a/Projects/Solar_Powered_Battery/Docs/Solar_Panel_Specs.xlsx
+++ b/Projects/Solar_Powered_Battery/Docs/Solar_Panel_Specs.xlsx
@@ -1,18 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21425"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF91B06A-CE8E-45CC-80FB-0C67C25E71E7}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Output_Power" sheetId="1" r:id="rId1"/>
     <sheet name="Calculation" sheetId="2" r:id="rId2"/>
     <sheet name="ToDo" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -312,9 +311,9 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="0.000"/>
+    <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -388,13 +387,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -409,9 +402,15 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -427,9 +426,9 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="de-DE"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -466,7 +465,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="de-DE"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -809,7 +808,7 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-41FC-4065-8FD8-7B09B5829832}"/>
             </c:ext>
@@ -823,11 +822,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="390091672"/>
-        <c:axId val="390092456"/>
+        <c:axId val="370451264"/>
+        <c:axId val="370452440"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="390091672"/>
+        <c:axId val="370451264"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -881,15 +880,15 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="390092456"/>
+        <c:crossAx val="370452440"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="390092456"/>
+        <c:axId val="370452440"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -943,10 +942,10 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="390091672"/>
+        <c:crossAx val="370451264"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -960,14 +959,14 @@
     </c:plotArea>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
-    <c:extLst>
+    <c:showDLblsOverMax val="0"/>
+    <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
       <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
         <c16r3:dataDisplayOptions16>
           <c16r3:dispNaAsBlank val="1"/>
         </c16r3:dataDisplayOptions16>
       </c:ext>
     </c:extLst>
-    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -991,7 +990,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="de-DE"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -1578,7 +1577,7 @@
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{335F42FB-C32E-4F1A-A28F-21DAE6D43FE9}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{335F42FB-C32E-4F1A-A28F-21DAE6D43FE9}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1619,7 +1618,7 @@
         <xdr:cNvPr id="2" name="Rechteck 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1746,7 +1745,7 @@
         <xdr:cNvPr id="3" name="Rechteck 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000003000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1962,7 +1961,7 @@
         <xdr:cNvPr id="8" name="Gruppieren 7">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000008000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000008000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1981,7 +1980,7 @@
           <xdr:cNvPr id="5" name="Gleichschenkliges Dreieck 4">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000005000000}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000005000000}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -2034,7 +2033,7 @@
           <xdr:cNvPr id="7" name="Gerader Verbinder 6">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000007000000}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000007000000}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -2090,7 +2089,7 @@
         <xdr:cNvPr id="9" name="Gruppieren 8">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000009000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000009000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2109,7 +2108,7 @@
           <xdr:cNvPr id="10" name="Gleichschenkliges Dreieck 9">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-00000A000000}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-00000A000000}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -2162,7 +2161,7 @@
           <xdr:cNvPr id="11" name="Gerader Verbinder 10">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-00000B000000}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-00000B000000}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -2218,7 +2217,7 @@
         <xdr:cNvPr id="13" name="Gewinkelte Verbindung 12">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-00000D000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-00000D000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2278,7 +2277,7 @@
         <xdr:cNvPr id="14" name="Gewinkelte Verbindung 13">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-00000E000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-00000E000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2336,7 +2335,7 @@
         <xdr:cNvPr id="17" name="Gewinkelte Verbindung 16">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000011000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000011000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2396,7 +2395,7 @@
         <xdr:cNvPr id="20" name="Rechteck 19">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000014000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000014000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2530,7 +2529,7 @@
         <xdr:cNvPr id="28" name="Rechteck 27">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-00001C000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-00001C000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2590,7 +2589,7 @@
         <xdr:cNvPr id="31" name="Gewinkelte Verbindung 30">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-00001F000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-00001F000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2648,7 +2647,7 @@
         <xdr:cNvPr id="39" name="Gewinkelte Verbindung 38">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000027000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000027000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2706,7 +2705,7 @@
         <xdr:cNvPr id="51" name="Gewinkelte Verbindung 50">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000033000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000033000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2764,7 +2763,7 @@
         <xdr:cNvPr id="60" name="Rechteck 59">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-00003C000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-00003C000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2954,7 +2953,7 @@
         <xdr:cNvPr id="78" name="Rechteck 77">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-00004E000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-00004E000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3149,7 +3148,7 @@
         <xdr:cNvPr id="79" name="Gewinkelte Verbindung 50">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-00004F000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-00004F000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3207,7 +3206,7 @@
         <xdr:cNvPr id="82" name="Gewinkelte Verbindung 50">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000052000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000052000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3265,7 +3264,7 @@
         <xdr:cNvPr id="87" name="Rechteck 86">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000057000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000057000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3450,7 +3449,7 @@
         <xdr:cNvPr id="88" name="Gewinkelte Verbindung 50">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000058000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000058000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3508,7 +3507,7 @@
         <xdr:cNvPr id="97" name="Rechteck 96">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000061000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000061000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3670,7 +3669,7 @@
         <xdr:cNvPr id="98" name="Gewinkelte Verbindung 50">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000062000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000062000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3728,7 +3727,7 @@
         <xdr:cNvPr id="101" name="Gewinkelte Verbindung 50">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000065000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000065000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3786,7 +3785,7 @@
         <xdr:cNvPr id="27" name="Gruppieren 7">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FE9B4560-03B7-49D8-ABAA-6DF52D2E6FEC}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{FE9B4560-03B7-49D8-ABAA-6DF52D2E6FEC}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3805,7 +3804,7 @@
           <xdr:cNvPr id="29" name="Gleichschenkliges Dreieck 4">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{771D8A4A-94AB-4165-BC57-11AA9E434C28}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{771D8A4A-94AB-4165-BC57-11AA9E434C28}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -3858,7 +3857,7 @@
           <xdr:cNvPr id="30" name="Gerader Verbinder 6">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{148873E4-A367-4356-9A37-C2F4F6ED8066}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{148873E4-A367-4356-9A37-C2F4F6ED8066}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -3914,7 +3913,7 @@
         <xdr:cNvPr id="32" name="Gewinkelte Verbindung 50">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{83F7249D-5EA2-4D24-849F-0879697C9CB5}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{83F7249D-5EA2-4D24-849F-0879697C9CB5}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3972,7 +3971,7 @@
         <xdr:cNvPr id="22" name="Straight Arrow Connector 21">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B51CA21D-57CB-4ABB-84CD-BA74A5D962DE}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{B51CA21D-57CB-4ABB-84CD-BA74A5D962DE}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4275,14 +4274,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B54"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13.28515625" bestFit="1" customWidth="1"/>
   </cols>
@@ -4797,14 +4796,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S73"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A34" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A59" sqref="A59:C59"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="23.7109375" style="5" customWidth="1"/>
     <col min="2" max="3" width="11.42578125" style="3"/>
@@ -5026,18 +5025,18 @@
       </c>
     </row>
     <row r="32" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A32" s="6" t="s">
+      <c r="A32" s="12" t="s">
         <v>63</v>
       </c>
-      <c r="B32" s="6"/>
-      <c r="C32" s="6"/>
+      <c r="B32" s="12"/>
+      <c r="C32" s="12"/>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33" s="8" t="s">
+      <c r="A33" s="11" t="s">
         <v>80</v>
       </c>
-      <c r="B33" s="8"/>
-      <c r="C33" s="8"/>
+      <c r="B33" s="11"/>
+      <c r="C33" s="11"/>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" s="5" t="s">
@@ -5054,7 +5053,7 @@
       <c r="A35" s="5" t="s">
         <v>88</v>
       </c>
-      <c r="B35" s="7">
+      <c r="B35" s="6">
         <f>1.4+0.85</f>
         <v>2.25</v>
       </c>
@@ -5066,7 +5065,7 @@
       <c r="A36" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B36" s="7">
+      <c r="B36" s="6">
         <v>5</v>
       </c>
       <c r="C36" s="3" t="s">
@@ -5077,7 +5076,7 @@
       <c r="A37" s="5" t="s">
         <v>89</v>
       </c>
-      <c r="B37" s="7">
+      <c r="B37" s="6">
         <f>B35/B36</f>
         <v>0.45</v>
       </c>
@@ -5086,14 +5085,14 @@
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B38" s="7"/>
+      <c r="B38" s="6"/>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A39" s="8" t="s">
+      <c r="A39" s="11" t="s">
         <v>81</v>
       </c>
-      <c r="B39" s="8"/>
-      <c r="C39" s="8"/>
+      <c r="B39" s="11"/>
+      <c r="C39" s="11"/>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" s="5" t="s">
@@ -5145,17 +5144,17 @@
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A47" s="8" t="s">
+      <c r="A47" s="11" t="s">
         <v>82</v>
       </c>
-      <c r="B47" s="8"/>
-      <c r="C47" s="8"/>
+      <c r="B47" s="11"/>
+      <c r="C47" s="11"/>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="B48" s="7">
+      <c r="B48" s="6">
         <v>5</v>
       </c>
       <c r="C48" s="3" t="s">
@@ -5166,7 +5165,7 @@
       <c r="A49" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="B49" s="7">
+      <c r="B49" s="6">
         <f>B48*B40/B37</f>
         <v>10</v>
       </c>
@@ -5178,7 +5177,7 @@
       <c r="A50" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="B50" s="7">
+      <c r="B50" s="6">
         <f>B48/(B53*B54)</f>
         <v>37.037037037037038</v>
       </c>
@@ -5187,14 +5186,14 @@
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B51" s="7"/>
+      <c r="B51" s="6"/>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A52" s="8" t="s">
+      <c r="A52" s="11" t="s">
         <v>79</v>
       </c>
-      <c r="B52" s="8"/>
-      <c r="C52" s="8"/>
+      <c r="B52" s="11"/>
+      <c r="C52" s="11"/>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" s="5" t="s">
@@ -5216,11 +5215,11 @@
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A59" s="8" t="s">
+      <c r="A59" s="11" t="s">
         <v>83</v>
       </c>
-      <c r="B59" s="8"/>
-      <c r="C59" s="8"/>
+      <c r="B59" s="11"/>
+      <c r="C59" s="11"/>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" s="5" t="s">
@@ -5272,29 +5271,29 @@
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A66" s="12" t="s">
+      <c r="A66" s="10" t="s">
         <v>94</v>
       </c>
-      <c r="B66" s="7">
+      <c r="B66" s="6">
         <f>B37</f>
         <v>0.45</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A68" s="8" t="s">
+      <c r="A68" s="11" t="s">
         <v>90</v>
       </c>
-      <c r="B68" s="8"/>
-      <c r="C68" s="8"/>
+      <c r="B68" s="11"/>
+      <c r="C68" s="11"/>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A69" s="10" t="s">
+      <c r="A69" s="8" t="s">
         <v>91</v>
       </c>
-      <c r="B69" s="9">
+      <c r="B69" s="7">
         <v>0</v>
       </c>
-      <c r="C69" s="9" t="s">
+      <c r="C69" s="7" t="s">
         <v>67</v>
       </c>
     </row>
@@ -5336,7 +5335,7 @@
       <c r="A73" s="5" t="s">
         <v>89</v>
       </c>
-      <c r="B73" s="11" t="e">
+      <c r="B73" s="9" t="e">
         <f>B71/B69</f>
         <v>#DIV/0!</v>
       </c>
@@ -5361,14 +5360,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D62BF99-86B7-40C4-9F30-110AD341EFE4}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">

</xml_diff>

<commit_message>
add new solar panel schematic
</commit_message>
<xml_diff>
--- a/Projects/Solar_Powered_Battery/Docs/Solar_Panel_Specs.xlsx
+++ b/Projects/Solar_Powered_Battery/Docs/Solar_Panel_Specs.xlsx
@@ -1,17 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21425"/>
   <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5F74434-0F24-45B4-8279-A8EB21E14444}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1"/>
+    <workbookView xWindow="1560" yWindow="1560" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Output_Power" sheetId="1" r:id="rId1"/>
     <sheet name="Calculation" sheetId="2" r:id="rId2"/>
     <sheet name="ToDo" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="181029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -21,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="108">
   <si>
     <t>Pout_max[W]</t>
   </si>
@@ -306,12 +308,51 @@
   </si>
   <si>
     <t>Iout_min</t>
+  </si>
+  <si>
+    <t>V_EN</t>
+  </si>
+  <si>
+    <t>Vin_typ</t>
+  </si>
+  <si>
+    <t>R1</t>
+  </si>
+  <si>
+    <t>R2</t>
+  </si>
+  <si>
+    <t>Vref</t>
+  </si>
+  <si>
+    <t>Iref</t>
+  </si>
+  <si>
+    <t>VKA</t>
+  </si>
+  <si>
+    <t>Reference voltage TL431</t>
+  </si>
+  <si>
+    <t>EN</t>
+  </si>
+  <si>
+    <t>Vin</t>
+  </si>
+  <si>
+    <t>CFF</t>
+  </si>
+  <si>
+    <t>Ohm</t>
+  </si>
+  <si>
+    <t>F</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
@@ -331,7 +372,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -341,6 +382,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -372,7 +425,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -402,15 +455,31 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -426,9 +495,9 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="de-DE"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -465,7 +534,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="de-DE"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -808,7 +877,7 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-41FC-4065-8FD8-7B09B5829832}"/>
             </c:ext>
@@ -880,7 +949,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="de-DE"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="370452440"/>
@@ -942,7 +1011,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="de-DE"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="370451264"/>
@@ -959,14 +1028,14 @@
     </c:plotArea>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
-    <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+    <c:extLst>
       <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
         <c16r3:dataDisplayOptions16>
           <c16r3:dispNaAsBlank val="1"/>
         </c16r3:dataDisplayOptions16>
       </c:ext>
     </c:extLst>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -990,7 +1059,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="de-DE"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -1577,7 +1646,7 @@
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{335F42FB-C32E-4F1A-A28F-21DAE6D43FE9}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{335F42FB-C32E-4F1A-A28F-21DAE6D43FE9}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1618,7 +1687,7 @@
         <xdr:cNvPr id="2" name="Rechteck 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1745,7 +1814,7 @@
         <xdr:cNvPr id="3" name="Rechteck 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000003000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1961,7 +2030,7 @@
         <xdr:cNvPr id="8" name="Gruppieren 7">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000008000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000008000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1980,7 +2049,7 @@
           <xdr:cNvPr id="5" name="Gleichschenkliges Dreieck 4">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000005000000}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000005000000}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -2033,7 +2102,7 @@
           <xdr:cNvPr id="7" name="Gerader Verbinder 6">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000007000000}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000007000000}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -2089,7 +2158,7 @@
         <xdr:cNvPr id="9" name="Gruppieren 8">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000009000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000009000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2108,7 +2177,7 @@
           <xdr:cNvPr id="10" name="Gleichschenkliges Dreieck 9">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-00000A000000}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-00000A000000}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -2161,7 +2230,7 @@
           <xdr:cNvPr id="11" name="Gerader Verbinder 10">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-00000B000000}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-00000B000000}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -2217,7 +2286,7 @@
         <xdr:cNvPr id="13" name="Gewinkelte Verbindung 12">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-00000D000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-00000D000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2277,7 +2346,7 @@
         <xdr:cNvPr id="14" name="Gewinkelte Verbindung 13">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-00000E000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-00000E000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2335,7 +2404,7 @@
         <xdr:cNvPr id="17" name="Gewinkelte Verbindung 16">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000011000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000011000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2395,7 +2464,7 @@
         <xdr:cNvPr id="20" name="Rechteck 19">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000014000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000014000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2529,7 +2598,7 @@
         <xdr:cNvPr id="28" name="Rechteck 27">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-00001C000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-00001C000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2589,7 +2658,7 @@
         <xdr:cNvPr id="31" name="Gewinkelte Verbindung 30">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-00001F000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-00001F000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2647,7 +2716,7 @@
         <xdr:cNvPr id="39" name="Gewinkelte Verbindung 38">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000027000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000027000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2705,7 +2774,7 @@
         <xdr:cNvPr id="51" name="Gewinkelte Verbindung 50">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000033000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000033000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2763,7 +2832,7 @@
         <xdr:cNvPr id="60" name="Rechteck 59">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-00003C000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-00003C000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2953,7 +3022,7 @@
         <xdr:cNvPr id="78" name="Rechteck 77">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-00004E000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-00004E000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3148,7 +3217,7 @@
         <xdr:cNvPr id="79" name="Gewinkelte Verbindung 50">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-00004F000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-00004F000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3206,7 +3275,7 @@
         <xdr:cNvPr id="82" name="Gewinkelte Verbindung 50">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000052000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000052000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3264,7 +3333,7 @@
         <xdr:cNvPr id="87" name="Rechteck 86">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000057000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000057000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3449,7 +3518,7 @@
         <xdr:cNvPr id="88" name="Gewinkelte Verbindung 50">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000058000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000058000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3507,7 +3576,7 @@
         <xdr:cNvPr id="97" name="Rechteck 96">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000061000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000061000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3669,7 +3738,7 @@
         <xdr:cNvPr id="98" name="Gewinkelte Verbindung 50">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000062000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000062000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3727,7 +3796,7 @@
         <xdr:cNvPr id="101" name="Gewinkelte Verbindung 50">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000065000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000065000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3785,7 +3854,7 @@
         <xdr:cNvPr id="27" name="Gruppieren 7">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{FE9B4560-03B7-49D8-ABAA-6DF52D2E6FEC}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FE9B4560-03B7-49D8-ABAA-6DF52D2E6FEC}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3804,7 +3873,7 @@
           <xdr:cNvPr id="29" name="Gleichschenkliges Dreieck 4">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{771D8A4A-94AB-4165-BC57-11AA9E434C28}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{771D8A4A-94AB-4165-BC57-11AA9E434C28}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -3857,7 +3926,7 @@
           <xdr:cNvPr id="30" name="Gerader Verbinder 6">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{148873E4-A367-4356-9A37-C2F4F6ED8066}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{148873E4-A367-4356-9A37-C2F4F6ED8066}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -3913,7 +3982,7 @@
         <xdr:cNvPr id="32" name="Gewinkelte Verbindung 50">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{83F7249D-5EA2-4D24-849F-0879697C9CB5}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{83F7249D-5EA2-4D24-849F-0879697C9CB5}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3971,7 +4040,7 @@
         <xdr:cNvPr id="22" name="Straight Arrow Connector 21">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{B51CA21D-57CB-4ABB-84CD-BA74A5D962DE}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B51CA21D-57CB-4ABB-84CD-BA74A5D962DE}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4007,6 +4076,94 @@
         </a:fontRef>
       </xdr:style>
     </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>737152</xdr:colOff>
+      <xdr:row>82</xdr:row>
+      <xdr:rowOff>107077</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>380572</xdr:colOff>
+      <xdr:row>93</xdr:row>
+      <xdr:rowOff>77767</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6B6085F1-0D52-4658-B9CF-F7380C79829F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3081130" y="15728077"/>
+          <a:ext cx="3453420" cy="2066190"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>223631</xdr:colOff>
+      <xdr:row>64</xdr:row>
+      <xdr:rowOff>184296</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>339683</xdr:colOff>
+      <xdr:row>67</xdr:row>
+      <xdr:rowOff>98055</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="Picture 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{25380524-C71C-4F87-A0DD-7D27181B6D71}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5615609" y="12376296"/>
+          <a:ext cx="1640052" cy="485259"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -4274,14 +4431,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B54"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13.28515625" bestFit="1" customWidth="1"/>
   </cols>
@@ -4796,14 +4953,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S73"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:S86"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B46" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="H63" sqref="H63"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="23.7109375" style="5" customWidth="1"/>
     <col min="2" max="3" width="11.42578125" style="3"/>
@@ -5025,18 +5182,18 @@
       </c>
     </row>
     <row r="32" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A32" s="12" t="s">
+      <c r="A32" s="13" t="s">
         <v>63</v>
       </c>
-      <c r="B32" s="12"/>
-      <c r="C32" s="12"/>
+      <c r="B32" s="13"/>
+      <c r="C32" s="13"/>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33" s="11" t="s">
+      <c r="A33" s="12" t="s">
         <v>80</v>
       </c>
-      <c r="B33" s="11"/>
-      <c r="C33" s="11"/>
+      <c r="B33" s="12"/>
+      <c r="C33" s="12"/>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" s="5" t="s">
@@ -5088,11 +5245,11 @@
       <c r="B38" s="6"/>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A39" s="11" t="s">
+      <c r="A39" s="12" t="s">
         <v>81</v>
       </c>
-      <c r="B39" s="11"/>
-      <c r="C39" s="11"/>
+      <c r="B39" s="12"/>
+      <c r="C39" s="12"/>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" s="5" t="s">
@@ -5106,6 +5263,9 @@
       <c r="A41" s="5" t="s">
         <v>85</v>
       </c>
+      <c r="B41" s="3">
+        <v>2</v>
+      </c>
       <c r="C41" s="3" t="s">
         <v>67</v>
       </c>
@@ -5114,6 +5274,9 @@
       <c r="A42" s="5" t="s">
         <v>86</v>
       </c>
+      <c r="B42" s="3">
+        <v>24</v>
+      </c>
       <c r="C42" s="3" t="s">
         <v>67</v>
       </c>
@@ -5122,6 +5285,9 @@
       <c r="A43" s="5" t="s">
         <v>2</v>
       </c>
+      <c r="B43" s="3">
+        <v>5</v>
+      </c>
       <c r="C43" s="3" t="s">
         <v>67</v>
       </c>
@@ -5130,6 +5296,9 @@
       <c r="A44" s="5" t="s">
         <v>3</v>
       </c>
+      <c r="B44" s="3">
+        <v>4</v>
+      </c>
       <c r="C44" s="3" t="s">
         <v>68</v>
       </c>
@@ -5140,218 +5309,411 @@
       </c>
       <c r="B45" s="3">
         <f>B43+B44</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A47" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="C45" s="3" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A46" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="B46" s="11">
+        <v>1.5</v>
+      </c>
+      <c r="C46" s="11" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A48" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="B47" s="11"/>
-      <c r="C47" s="11"/>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A48" s="5" t="s">
+      <c r="B48" s="12"/>
+      <c r="C48" s="12"/>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A49" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="B48" s="6">
+      <c r="B49" s="6">
         <v>5</v>
       </c>
-      <c r="C48" s="3" t="s">
+      <c r="C49" s="3" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A49" s="5" t="s">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A50" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="B49" s="6">
-        <f>B48*B40/B37</f>
+      <c r="B50" s="6">
+        <f>B49*B40/B37</f>
         <v>10</v>
-      </c>
-      <c r="C49" s="3" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A50" s="5" t="s">
-        <v>77</v>
-      </c>
-      <c r="B50" s="6">
-        <f>B48/(B53*B54)</f>
-        <v>37.037037037037038</v>
       </c>
       <c r="C50" s="3" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B51" s="6"/>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A52" s="11" t="s">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A51" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="B51" s="6">
+        <f>B49/(B58*B59)</f>
+        <v>37.037037037037038</v>
+      </c>
+      <c r="C51" s="3" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B52" s="6"/>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A53" s="12" t="s">
         <v>79</v>
       </c>
-      <c r="B52" s="11"/>
-      <c r="C52" s="11"/>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A53" s="5" t="s">
+      <c r="B53" s="12"/>
+      <c r="C53" s="12"/>
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A54" s="14" t="s">
+        <v>85</v>
+      </c>
+      <c r="B54" s="7">
+        <v>4</v>
+      </c>
+      <c r="C54" s="7" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A55" s="14" t="s">
+        <v>96</v>
+      </c>
+      <c r="B55" s="7">
+        <v>5</v>
+      </c>
+      <c r="C55" s="7" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A56" s="14" t="s">
+        <v>86</v>
+      </c>
+      <c r="B56" s="7">
+        <v>8</v>
+      </c>
+      <c r="C56" s="7" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A57" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="B57" s="7">
+        <v>4.2</v>
+      </c>
+      <c r="C57" s="7" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A58" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="B53" s="3">
+      <c r="B58" s="3">
         <v>0.9</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A54" s="5" t="s">
+    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A59" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="B54" s="3">
+      <c r="B59" s="9">
         <v>0.15</v>
       </c>
-      <c r="C54" s="3" t="s">
+      <c r="C59" s="3" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A59" s="11" t="s">
+    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A61" s="12" t="s">
         <v>83</v>
       </c>
-      <c r="B59" s="11"/>
-      <c r="C59" s="11"/>
-    </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A60" s="5" t="s">
+      <c r="B61" s="12"/>
+      <c r="C61" s="12"/>
+      <c r="D61" s="17" t="s">
+        <v>103</v>
+      </c>
+      <c r="E61" s="17"/>
+      <c r="F61" s="17"/>
+      <c r="G61" s="18" t="s">
+        <v>105</v>
+      </c>
+      <c r="H61" s="18"/>
+      <c r="I61" s="18"/>
+    </row>
+    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A62" s="5" t="s">
         <v>84</v>
       </c>
-      <c r="B60" s="3">
+      <c r="B62" s="3">
         <v>0.9</v>
       </c>
-    </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A61" s="5" t="s">
+      <c r="D62" t="s">
+        <v>104</v>
+      </c>
+      <c r="E62">
+        <v>5.5</v>
+      </c>
+      <c r="F62" t="s">
+        <v>67</v>
+      </c>
+      <c r="G62" t="s">
+        <v>97</v>
+      </c>
+      <c r="H62" s="16">
+        <v>6200</v>
+      </c>
+      <c r="I62" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A63" s="5" t="s">
         <v>85</v>
       </c>
-      <c r="C61" s="3" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A62" s="5" t="s">
-        <v>86</v>
-      </c>
-      <c r="C62" s="3" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A63" s="5" t="s">
-        <v>2</v>
+      <c r="B63" s="3">
+        <v>3.6</v>
       </c>
       <c r="C63" s="3" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D63" t="s">
+        <v>95</v>
+      </c>
+      <c r="E63">
+        <v>1.3</v>
+      </c>
+      <c r="G63" t="s">
+        <v>105</v>
+      </c>
+      <c r="H63">
+        <f>1/(31000*H62)</f>
+        <v>5.2029136316337152E-9</v>
+      </c>
+      <c r="I63" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A64" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="B64" s="3">
+        <v>28</v>
+      </c>
+      <c r="C64" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="D64" t="s">
+        <v>97</v>
+      </c>
+      <c r="E64" s="16">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A65" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B65" s="3">
+        <v>5</v>
+      </c>
+      <c r="C65" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="D65" t="s">
+        <v>98</v>
+      </c>
+      <c r="E65">
+        <f>E64*(E62-E63)/E63</f>
+        <v>32307.692307692305</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A66" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="C64" s="3" t="s">
+      <c r="B66" s="3">
+        <v>3</v>
+      </c>
+      <c r="C66" s="3" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A65" s="5" t="s">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A67" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="B65" s="3">
-        <f>B63+B64</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A66" s="10" t="s">
+      <c r="B67" s="3">
+        <f>B65+B66</f>
+        <v>8</v>
+      </c>
+      <c r="C67" s="3" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A68" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="B68" s="11">
+        <v>1.2</v>
+      </c>
+      <c r="C68" s="11" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A69" s="10" t="s">
         <v>94</v>
       </c>
-      <c r="B66" s="6">
+      <c r="B69" s="6">
         <f>B37</f>
         <v>0.45</v>
       </c>
     </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A68" s="11" t="s">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A71" s="12" t="s">
         <v>90</v>
       </c>
-      <c r="B68" s="11"/>
-      <c r="C68" s="11"/>
-    </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A69" s="8" t="s">
+      <c r="B71" s="12"/>
+      <c r="C71" s="12"/>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A72" s="8" t="s">
         <v>91</v>
       </c>
-      <c r="B69" s="7">
+      <c r="B72" s="7">
         <v>0</v>
       </c>
-      <c r="C69" s="7" t="s">
+      <c r="C72" s="7" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A70" s="5" t="s">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A73" s="5" t="s">
         <v>92</v>
       </c>
-      <c r="B70" s="3">
+      <c r="B73" s="3">
         <v>12</v>
       </c>
-      <c r="C70" s="3" t="s">
+      <c r="C73" s="3" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A71" s="5" t="s">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A74" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="B71" s="3">
+      <c r="B74" s="3">
         <v>1.5</v>
       </c>
-      <c r="C71" s="3" t="s">
+      <c r="C74" s="3" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A72" s="5" t="s">
+    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A75" s="5" t="s">
         <v>93</v>
       </c>
-      <c r="B72" s="3">
-        <f>B71/B70</f>
+      <c r="B75" s="3">
+        <f>B74/B73</f>
         <v>0.125</v>
       </c>
-      <c r="C72" s="3" t="s">
+      <c r="C75" s="3" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A73" s="5" t="s">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A76" s="5" t="s">
         <v>89</v>
       </c>
-      <c r="B73" s="9" t="e">
-        <f>B71/B69</f>
+      <c r="B76" s="9" t="e">
+        <f>B74/B72</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="C73" s="3" t="s">
+      <c r="C76" s="3" t="s">
         <v>68</v>
       </c>
     </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A81" s="12" t="s">
+        <v>102</v>
+      </c>
+      <c r="B81" s="12"/>
+      <c r="C81" s="12"/>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A82" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="B82" s="15">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A83" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="B83" s="15">
+        <v>51000</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A84" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="B84" s="3">
+        <v>2.4950000000000001</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A85" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="B85" s="3">
+        <f>0.000004</f>
+        <v>3.9999999999999998E-6</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A86" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="B86" s="3">
+        <f>B84*(1+B82/B83)+B85*B82</f>
+        <v>3.02421568627451</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="7">
-    <mergeCell ref="A68:C68"/>
+  <mergeCells count="10">
+    <mergeCell ref="A81:C81"/>
+    <mergeCell ref="D61:F61"/>
+    <mergeCell ref="G61:I61"/>
+    <mergeCell ref="A71:C71"/>
     <mergeCell ref="A32:C32"/>
-    <mergeCell ref="A52:C52"/>
-    <mergeCell ref="A47:C47"/>
+    <mergeCell ref="A53:C53"/>
+    <mergeCell ref="A48:C48"/>
     <mergeCell ref="A39:C39"/>
     <mergeCell ref="A33:C33"/>
-    <mergeCell ref="A59:C59"/>
+    <mergeCell ref="A61:C61"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -5360,14 +5722,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">

</xml_diff>